<commit_message>
整合 lodash 和 mpath 的get，set方法到helper里
</commit_message>
<xml_diff>
--- a/test/controllers/i18n.xlsx
+++ b/test/controllers/i18n.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="4080" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="45780" yWindow="980" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -38,16 +38,15 @@
     <t>lang</t>
   </si>
   <si>
-    <t>test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>body</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>jp:a,en:b,zh:c</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r2space</t>
   </si>
 </sst>
 </file>
@@ -432,7 +431,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -453,13 +452,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>